<commit_message>
fixes handling integers and indexes in pandas
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK4"/>
+  <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,140 +745,6 @@
       <c r="BJ2" t="inlineStr"/>
       <c r="BK2" t="inlineStr"/>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr"/>
-      <c r="AV3" t="inlineStr"/>
-      <c r="AW3" t="inlineStr"/>
-      <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="inlineStr"/>
-      <c r="AZ3" t="inlineStr"/>
-      <c r="BA3" t="inlineStr"/>
-      <c r="BB3" t="inlineStr"/>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="inlineStr"/>
-      <c r="BE3" t="inlineStr"/>
-      <c r="BF3" t="inlineStr"/>
-      <c r="BG3" t="inlineStr"/>
-      <c r="BH3" t="inlineStr"/>
-      <c r="BI3" t="inlineStr"/>
-      <c r="BJ3" t="inlineStr"/>
-      <c r="BK3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="inlineStr"/>
-      <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="inlineStr"/>
-      <c r="AV4" t="inlineStr"/>
-      <c r="AW4" t="inlineStr"/>
-      <c r="AX4" t="inlineStr"/>
-      <c r="AY4" t="inlineStr"/>
-      <c r="AZ4" t="inlineStr"/>
-      <c r="BA4" t="inlineStr"/>
-      <c r="BB4" t="inlineStr"/>
-      <c r="BC4" t="inlineStr"/>
-      <c r="BD4" t="inlineStr"/>
-      <c r="BE4" t="inlineStr"/>
-      <c r="BF4" t="inlineStr"/>
-      <c r="BG4" t="inlineStr"/>
-      <c r="BH4" t="inlineStr"/>
-      <c r="BI4" t="inlineStr"/>
-      <c r="BJ4" t="inlineStr"/>
-      <c r="BK4" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>